<commit_message>
database testing test case
</commit_message>
<xml_diff>
--- a/Database Testing.xlsx
+++ b/Database Testing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pradip\Desktop\Mannual Testing Project\mero project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22E20432-B74F-4B3F-A978-A7ED2600864E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB7E4B39-7406-41D0-8F7E-6085422D6830}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{802CAE69-51C8-4C69-85B6-A402B4748F16}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="43">
   <si>
     <t>Database Testing</t>
   </si>
@@ -71,13 +71,105 @@
   </si>
   <si>
     <t>Status</t>
+  </si>
+  <si>
+    <t>TC0001</t>
+  </si>
+  <si>
+    <t>TC0002</t>
+  </si>
+  <si>
+    <t>TC0003</t>
+  </si>
+  <si>
+    <t>TC0004</t>
+  </si>
+  <si>
+    <t>TC0005</t>
+  </si>
+  <si>
+    <t>TC0006</t>
+  </si>
+  <si>
+    <t>TC0007</t>
+  </si>
+  <si>
+    <t>TC0008</t>
+  </si>
+  <si>
+    <t>Check Table Present in database schema</t>
+  </si>
+  <si>
+    <t>Check Table Name Conventions</t>
+  </si>
+  <si>
+    <t>Check Number of Columns in Table</t>
+  </si>
+  <si>
+    <t>Check Column Name in Table</t>
+  </si>
+  <si>
+    <t>Check Data Type of Column in Table</t>
+  </si>
+  <si>
+    <t>Check size of Column in Table</t>
+  </si>
+  <si>
+    <t>Check Null fields in Table</t>
+  </si>
+  <si>
+    <t>Check Column Keys in Table</t>
+  </si>
+  <si>
+    <t>shows tables;</t>
+  </si>
+  <si>
+    <t>select Count(*) AS NumberofColumn FROM 
+information_schema.columns WHERE table_name="customers";</t>
+  </si>
+  <si>
+    <t>select column_name FROM 
+information_schema.columns WHERE table_name="customers";</t>
+  </si>
+  <si>
+    <t>select column_name,data_type FROM 
+information_schema.columns WHERE table_name="customers";</t>
+  </si>
+  <si>
+    <t>select column_name,column_type FROM 
+information_schema.columns WHERE table_name="customers";</t>
+  </si>
+  <si>
+    <t>select column_name, is_nullable FROM 
+information_schema.columns WHERE table_name="customers";</t>
+  </si>
+  <si>
+    <t>select column_name, column_key FROM 
+information_schema.columns WHERE table_name="customers";</t>
+  </si>
+  <si>
+    <t>Table Name should 
+be displayed in the list</t>
+  </si>
+  <si>
+    <t>Table Name should 
+be single word. Shouldn't contain space</t>
+  </si>
+  <si>
+    <t>As mentioned in the Database Design</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>P1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -115,8 +207,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -133,6 +246,11 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -143,25 +261,31 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="3" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Good" xfId="3" builtinId="26"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -518,58 +642,220 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE0224B5-4775-4BFA-B2CC-2292FDE069EF}">
-  <dimension ref="A2:L4"/>
+  <dimension ref="A2:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="68.28515625" customWidth="1"/>
+    <col min="4" max="4" width="33.7109375" customWidth="1"/>
     <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:12" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
       <c r="F2" s="4"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+    </row>
+    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="7" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7">
+        <v>13</v>
+      </c>
+      <c r="F7" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G12" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -577,6 +863,8 @@
     <mergeCell ref="F2:L2"/>
     <mergeCell ref="B2:E2"/>
   </mergeCells>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>